<commit_message>
Update Purchase Entries Template with Debit Note Voucher Type
</commit_message>
<xml_diff>
--- a/Additional Libraries/Templates/Resources/PurchaseEntries.xlsx
+++ b/Additional Libraries/Templates/Resources/PurchaseEntries.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Dineshkumar\Projects\Excel-to-Tally-for-GST\E2TGST\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Dineshkumar\Projects\Excel-to-Tally-for-GST\Additional Libraries\Templates\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Invoice No</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>GSTIN/Party Ledger Name</t>
+  </si>
+  <si>
+    <t>Debit Note</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
   <dimension ref="A1:M1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1048576"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +518,7 @@
     <col min="8" max="8" width="14.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" style="3" customWidth="1"/>
     <col min="10" max="10" width="19" style="1" customWidth="1"/>
-    <col min="11" max="13" width="0" style="1" hidden="1"/>
+    <col min="11" max="13" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
@@ -4640,7 +4643,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$B$2:$B$6</xm:f>
+            <xm:f>Lists!$B$2:$B$8</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1001</xm:sqref>
         </x14:dataValidation>
@@ -4659,10 +4662,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Lists"/>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4720,8 +4723,13 @@
         <v>14</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="3I9eoWRern4OcmTePoQKn0TBBGovSxGbKVduHPkIGTA1smkXpWawyozzpGLIM2B8qUyV+2bQDftAChPAfckO7g==" saltValue="m6GmIdYnMb7VCu43w2eT4w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Vu1kYGz7ZMZHCuvuWn+n42agZ8ciJani7m134xhKAhJdPDKCUE6hKZqpKGwEwijaxh3XyLXjKhbbFydyfPmz9Q==" saltValue="QI4vcMWdu8xCAQTPXgvdkQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Purchase Entries Template
</commit_message>
<xml_diff>
--- a/Additional Libraries/Templates/Resources/PurchaseEntries.xlsx
+++ b/Additional Libraries/Templates/Resources/PurchaseEntries.xlsx
@@ -505,9 +505,7 @@
   <sheetPr codeName="PurchaseEntries"/>
   <dimension ref="A1:N1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5651,7 +5649,7 @@
           <x14:formula1>
             <xm:f>Lists!$B$2:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:J1001</xm:sqref>
+          <xm:sqref>I2:I1001</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>